<commit_message>
Update stocks_data.xlsx with latest data
</commit_message>
<xml_diff>
--- a/stocks_data.xlsx
+++ b/stocks_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA324E3-82E7-4154-A6D5-D2853F9BF728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E10F18C-9DE3-4FBB-9CFD-F7303730BAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1272,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10989,5 +10989,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>